<commit_message>
Proyecto de Clase. BBDD - DDL - Sentencias
</commit_message>
<xml_diff>
--- a/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
+++ b/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="S.I.W.Ventas" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>No tengo el producto</t>
-  </si>
-  <si>
-    <t>Reunión Vendedores</t>
   </si>
   <si>
     <t>PEDIDOS</t>
@@ -193,9 +190,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">No puede haber pedidos solo con el vendedor. </t>
-  </si>
-  <si>
     <t>RESTRICCIONES</t>
   </si>
   <si>
@@ -467,9 +461,6 @@
     <t>La existencia de un Pedido, depende del customer</t>
   </si>
   <si>
-    <t>Solo existe máximo un vendedor y un customer en un Pedido</t>
-  </si>
-  <si>
     <t>seller-2</t>
   </si>
   <si>
@@ -489,12 +480,21 @@
   </si>
   <si>
     <t>Un Mensaje puede ser escrito por Un Usuario. Un Usuario puede escribir Muchos Mensajes</t>
+  </si>
+  <si>
+    <t>Solo existe máximo un seller y un customer en un Pedido</t>
+  </si>
+  <si>
+    <t>Reunión selleres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No puede haber pedidos solo con el seller. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -1384,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1403,7 @@
     <row r="2" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="34"/>
       <c r="J3" s="10"/>
@@ -1444,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J6" s="10"/>
     </row>
@@ -1453,7 +1453,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -1462,13 +1462,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -1486,13 +1486,13 @@
         <v>21</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G10" s="63"/>
       <c r="I10" s="3"/>
@@ -1523,7 +1523,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12" s="1">
         <v>654321</v>
@@ -1543,7 +1543,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1">
         <v>987654</v>
@@ -1563,7 +1563,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D14" s="4">
         <v>654789</v>
@@ -1583,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1">
         <v>147852</v>
@@ -1623,7 +1623,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D17" s="48">
         <v>654321</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="18" spans="2:11" s="18" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="19" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="34"/>
@@ -1664,13 +1664,13 @@
         <v>22</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="15"/>
@@ -1688,7 +1688,7 @@
         <v>12345</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="15"/>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="49" t="s">
         <v>12</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="49" t="s">
         <v>13</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="25" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="26" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C28" s="21">
         <v>44788</v>
@@ -1795,13 +1795,13 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C29" s="21">
         <v>44800</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>28</v>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C30" s="21">
         <v>44800</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" s="26">
         <v>44804</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="25">
         <v>44800</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="33" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="20"/>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="34" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B34" s="32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="34"/>
       <c r="D34" s="3"/>
@@ -1876,13 +1876,13 @@
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="41" t="s">
         <v>22</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H35"/>
       <c r="I35"/>
@@ -1890,13 +1890,13 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G36" s="47"/>
       <c r="H36"/>
@@ -1905,13 +1905,13 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="E37" s="16"/>
       <c r="G37" s="18"/>
@@ -1921,13 +1921,13 @@
     </row>
     <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E38" s="16"/>
       <c r="G38" s="18"/>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="39" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B39" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
@@ -1951,22 +1951,22 @@
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I40" s="10"/>
       <c r="K40" s="2"/>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="21">
         <v>44774</v>
@@ -1991,7 +1991,7 @@
         <v>618800</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I41" s="10"/>
       <c r="K41" s="2"/>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" s="21">
         <v>44774</v>
@@ -2016,7 +2016,7 @@
         <v>178500</v>
       </c>
       <c r="G42" s="68" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I42" s="10"/>
       <c r="K42" s="2"/>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C43" s="21">
         <v>44803</v>
@@ -2041,7 +2041,7 @@
         <v>273700</v>
       </c>
       <c r="G43" s="69" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I43" s="10"/>
       <c r="K43" s="2"/>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="44" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" s="25">
         <v>44819</v>
@@ -2066,7 +2066,7 @@
         <v>95200</v>
       </c>
       <c r="G44" s="69" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="10"/>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="45" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="20"/>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="46" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B46" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" s="33"/>
       <c r="D46" s="34"/>
@@ -2098,13 +2098,13 @@
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D47" s="41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E47" s="35"/>
       <c r="G47" s="18"/>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="48" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D48" s="7">
         <v>5</v>
@@ -2129,10 +2129,10 @@
     </row>
     <row r="49" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D49" s="7">
         <v>1</v>
@@ -2144,10 +2144,10 @@
     </row>
     <row r="50" spans="2:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D50" s="9">
         <v>3</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="51" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B51" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
@@ -2174,22 +2174,22 @@
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C52" s="64" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F52" s="39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H52" s="63"/>
       <c r="I52" s="10"/>
@@ -2203,10 +2203,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D53" s="51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E53" s="52">
         <v>2500</v>
@@ -2215,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H53" s="60"/>
       <c r="I53" s="10"/>
@@ -2229,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D54" s="51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E54" s="52">
         <v>6500</v>
@@ -2241,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H54" s="61"/>
       <c r="I54" s="10"/>
@@ -2255,10 +2255,10 @@
         <v>2</v>
       </c>
       <c r="C55" s="65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D55" s="51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E55" s="52">
         <v>3500</v>
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H55" s="61"/>
       <c r="I55" s="10"/>
@@ -2281,10 +2281,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="66" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D56" s="55" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E56" s="56">
         <v>4500</v>
@@ -2293,7 +2293,7 @@
         <v>250</v>
       </c>
       <c r="G56" s="57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H56" s="61"/>
       <c r="I56" s="16"/>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="57" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="20"/>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="58" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B58" s="30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="3"/>
@@ -2327,10 +2327,10 @@
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C59" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D59" s="35"/>
       <c r="F59" s="46"/>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="46"/>
@@ -2356,7 +2356,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -2368,7 +2368,7 @@
         <v>3</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>

</xml_diff>

<commit_message>
Proyecto de Clase. BBDD - DML - Sentencias
</commit_message>
<xml_diff>
--- a/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
+++ b/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="109">
   <si>
     <t>admin</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Ramos</t>
-  </si>
-  <si>
-    <t>albeiro@</t>
   </si>
   <si>
     <t>admin-1</t>
@@ -489,6 +486,15 @@
   </si>
   <si>
     <t>Un Rol es asignado Muchas personas. Una persona se le asigna Un Rol</t>
+  </si>
+  <si>
+    <t>Alejandra</t>
+  </si>
+  <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>profealbeiro2020@</t>
   </si>
 </sst>
 </file>
@@ -1434,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1459,7 @@
     <row r="2" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -1466,17 +1472,17 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="34"/>
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="10"/>
     </row>
@@ -1494,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="10"/>
     </row>
@@ -1503,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -1512,13 +1518,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="76"/>
       <c r="D9" s="33"/>
@@ -1530,19 +1536,19 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>21</v>
-      </c>
       <c r="D10" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="37" t="s">
         <v>85</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>86</v>
       </c>
       <c r="G10" s="63"/>
       <c r="I10" s="3"/>
@@ -1553,16 +1559,16 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1">
         <v>123456</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G11" s="59"/>
       <c r="I11" s="3"/>
@@ -1573,7 +1579,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="77">
         <v>654321</v>
@@ -1593,7 +1599,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1">
         <v>987654</v>
@@ -1613,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="4">
         <v>654789</v>
@@ -1633,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1">
         <v>147852</v>
@@ -1653,16 +1659,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="13">
         <v>456987</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G16" s="59"/>
       <c r="I16" s="3"/>
@@ -1673,16 +1679,16 @@
         <v>4</v>
       </c>
       <c r="C17" s="71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="71">
-        <v>654321</v>
+        <v>555333</v>
       </c>
       <c r="E17" s="71" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="F17" s="72" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G17" s="59"/>
       <c r="I17" s="3"/>
@@ -1690,7 +1696,7 @@
     </row>
     <row r="18" spans="2:11" s="18" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
@@ -1700,7 +1706,7 @@
     </row>
     <row r="19" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="34"/>
@@ -1711,16 +1717,16 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="37" t="s">
-        <v>44</v>
-      </c>
       <c r="E20" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="15"/>
@@ -1729,16 +1735,16 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="D21" s="7">
         <v>12345</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="15"/>
@@ -1747,7 +1753,7 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" s="49" t="s">
         <v>12</v>
@@ -1763,7 +1769,7 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="49" t="s">
         <v>13</v>
@@ -1779,10 +1785,10 @@
     </row>
     <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D24" s="9">
         <v>12345</v>
@@ -1795,7 +1801,7 @@
     </row>
     <row r="25" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
@@ -1806,7 +1812,7 @@
     </row>
     <row r="26" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
@@ -1815,97 +1821,97 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="E27" s="37" t="s">
         <v>25</v>
-      </c>
-      <c r="E27" s="37" t="s">
-        <v>26</v>
       </c>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="21">
         <v>44788</v>
       </c>
       <c r="D28" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="21">
         <v>44800</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="21">
         <v>44800</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" s="26">
         <v>44804</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="25">
         <v>44800</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="20"/>
@@ -1916,7 +1922,7 @@
     </row>
     <row r="34" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B34" s="32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="34"/>
       <c r="D34" s="3"/>
@@ -1926,13 +1932,13 @@
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H35"/>
       <c r="I35"/>
@@ -1940,13 +1946,13 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="G36" s="47"/>
       <c r="H36"/>
@@ -1955,13 +1961,13 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E37" s="16"/>
       <c r="G37" s="18"/>
@@ -1971,13 +1977,13 @@
     </row>
     <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38" s="16"/>
       <c r="G38" s="18"/>
@@ -1987,7 +1993,7 @@
     </row>
     <row r="39" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B39" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
@@ -2001,22 +2007,22 @@
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="39" t="s">
+      <c r="F40" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F40" s="37" t="s">
-        <v>49</v>
-      </c>
       <c r="G40" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I40" s="10"/>
       <c r="K40" s="2"/>
@@ -2024,7 +2030,7 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="21">
         <v>44774</v>
@@ -2041,7 +2047,7 @@
         <v>618800</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I41" s="10"/>
       <c r="K41" s="2"/>
@@ -2049,7 +2055,7 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="21">
         <v>44774</v>
@@ -2066,7 +2072,7 @@
         <v>178500</v>
       </c>
       <c r="G42" s="68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I42" s="10"/>
       <c r="K42" s="2"/>
@@ -2074,7 +2080,7 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="21">
         <v>44803</v>
@@ -2091,7 +2097,7 @@
         <v>273700</v>
       </c>
       <c r="G43" s="69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I43" s="10"/>
       <c r="K43" s="2"/>
@@ -2099,7 +2105,7 @@
     </row>
     <row r="44" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" s="25">
         <v>44819</v>
@@ -2116,7 +2122,7 @@
         <v>95200</v>
       </c>
       <c r="G44" s="69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="10"/>
@@ -2125,7 +2131,7 @@
     </row>
     <row r="45" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="20"/>
@@ -2136,7 +2142,7 @@
     </row>
     <row r="46" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B46" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C46" s="33"/>
       <c r="D46" s="34"/>
@@ -2148,13 +2154,13 @@
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D47" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E47" s="35"/>
       <c r="G47" s="18"/>
@@ -2164,10 +2170,10 @@
     </row>
     <row r="48" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" s="7">
         <v>5</v>
@@ -2179,10 +2185,10 @@
     </row>
     <row r="49" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="7">
         <v>1</v>
@@ -2194,10 +2200,10 @@
     </row>
     <row r="50" spans="2:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" s="9">
         <v>3</v>
@@ -2209,7 +2215,7 @@
     </row>
     <row r="51" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B51" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
@@ -2224,22 +2230,22 @@
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="38" t="s">
-        <v>60</v>
-      </c>
       <c r="E52" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F52" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G52" s="37" t="s">
         <v>69</v>
-      </c>
-      <c r="G52" s="37" t="s">
-        <v>70</v>
       </c>
       <c r="H52" s="63"/>
       <c r="I52" s="10"/>
@@ -2253,10 +2259,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D53" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" s="52">
         <v>2500</v>
@@ -2265,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H53" s="60"/>
       <c r="I53" s="10"/>
@@ -2279,10 +2285,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E54" s="52">
         <v>6500</v>
@@ -2291,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H54" s="61"/>
       <c r="I54" s="10"/>
@@ -2305,10 +2311,10 @@
         <v>2</v>
       </c>
       <c r="C55" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D55" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E55" s="52">
         <v>3500</v>
@@ -2317,7 +2323,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H55" s="61"/>
       <c r="I55" s="10"/>
@@ -2331,10 +2337,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="55" t="s">
         <v>64</v>
-      </c>
-      <c r="D56" s="55" t="s">
-        <v>65</v>
       </c>
       <c r="E56" s="56">
         <v>4500</v>
@@ -2343,7 +2349,7 @@
         <v>250</v>
       </c>
       <c r="G56" s="57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H56" s="61"/>
       <c r="I56" s="16"/>
@@ -2354,7 +2360,7 @@
     </row>
     <row r="57" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="20"/>
@@ -2365,7 +2371,7 @@
     </row>
     <row r="58" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B58" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="3"/>
@@ -2377,10 +2383,10 @@
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="41" t="s">
         <v>72</v>
-      </c>
-      <c r="C59" s="41" t="s">
-        <v>73</v>
       </c>
       <c r="D59" s="35"/>
       <c r="F59" s="46"/>
@@ -2394,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="46"/>
@@ -2406,7 +2412,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -2418,7 +2424,7 @@
         <v>3</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>

</xml_diff>

<commit_message>
Proyecto de Clase. Ajustando BBDD - MR
</commit_message>
<xml_diff>
--- a/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
+++ b/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\adsi_n-2395871_g3\assets\docs\Trim3\Trim3_Ev1-ModeloRelacional\Trim3_Ev1_1-Normalización\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7B8861-0980-48AA-8F34-253068C05A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S.I.W.Ventas" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -500,9 +509,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -923,7 +932,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1048,16 +1057,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1437,26 +1446,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="10" customWidth="1"/>
-    <col min="2" max="6" width="25.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="46" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="10" customWidth="1"/>
+    <col min="2" max="6" width="25.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="46" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="1.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
       <c r="B2" s="16" t="s">
         <v>105</v>
@@ -1470,14 +1479,14 @@
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="32" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="34"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
@@ -1486,7 +1495,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>1</v>
       </c>
@@ -1495,7 +1504,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>2</v>
       </c>
@@ -1504,7 +1513,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1513,7 +1522,7 @@
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1522,7 +1531,7 @@
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B9" s="75" t="s">
         <v>83</v>
       </c>
@@ -1534,7 +1543,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="36" t="s">
         <v>19</v>
       </c>
@@ -1554,7 +1563,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>1</v>
       </c>
@@ -1574,7 +1583,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="73">
         <v>3</v>
       </c>
@@ -1594,7 +1603,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>4</v>
       </c>
@@ -1614,7 +1623,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>2</v>
       </c>
@@ -1634,7 +1643,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>2</v>
       </c>
@@ -1654,7 +1663,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="29">
         <v>1</v>
       </c>
@@ -1674,7 +1683,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="70">
         <v>4</v>
       </c>
@@ -1694,7 +1703,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="2:11" s="18" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" s="18" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="18" t="s">
         <v>100</v>
       </c>
@@ -1704,7 +1713,7 @@
       <c r="G18" s="20"/>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B19" s="32" t="s">
         <v>32</v>
       </c>
@@ -1715,7 +1724,7 @@
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="36" t="s">
         <v>21</v>
       </c>
@@ -1733,7 +1742,7 @@
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
@@ -1751,7 +1760,7 @@
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>94</v>
       </c>
@@ -1767,7 +1776,7 @@
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>90</v>
       </c>
@@ -1783,7 +1792,7 @@
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
         <v>17</v>
       </c>
@@ -1799,7 +1808,7 @@
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="18" t="s">
         <v>101</v>
       </c>
@@ -1810,7 +1819,7 @@
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B26" s="32" t="s">
         <v>33</v>
       </c>
@@ -1819,7 +1828,7 @@
       <c r="E26" s="34"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="36" t="s">
         <v>21</v>
       </c>
@@ -1834,7 +1843,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>97</v>
       </c>
@@ -1849,7 +1858,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>98</v>
       </c>
@@ -1864,7 +1873,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
         <v>98</v>
       </c>
@@ -1879,7 +1888,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="29" t="s">
         <v>94</v>
       </c>
@@ -1894,7 +1903,7 @@
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="11" t="s">
         <v>94</v>
       </c>
@@ -1909,7 +1918,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
         <v>38</v>
       </c>
@@ -1920,7 +1929,7 @@
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B34" s="32" t="s">
         <v>88</v>
       </c>
@@ -1930,7 +1939,7 @@
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="40" t="s">
         <v>35</v>
       </c>
@@ -1944,7 +1953,7 @@
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
         <v>36</v>
       </c>
@@ -1959,7 +1968,7 @@
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="6" t="s">
         <v>36</v>
       </c>
@@ -1975,7 +1984,7 @@
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="8" t="s">
         <v>37</v>
       </c>
@@ -1991,7 +2000,7 @@
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B39" s="32" t="s">
         <v>30</v>
       </c>
@@ -2005,7 +2014,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="36" t="s">
         <v>41</v>
       </c>
@@ -2028,7 +2037,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="6" t="s">
         <v>34</v>
       </c>
@@ -2053,7 +2062,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
         <v>46</v>
       </c>
@@ -2078,7 +2087,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
         <v>50</v>
       </c>
@@ -2103,7 +2112,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="11" t="s">
         <v>49</v>
       </c>
@@ -2129,7 +2138,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="18" t="s">
         <v>81</v>
       </c>
@@ -2140,7 +2149,7 @@
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B46" s="32" t="s">
         <v>89</v>
       </c>
@@ -2152,7 +2161,7 @@
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="40" t="s">
         <v>35</v>
       </c>
@@ -2168,7 +2177,7 @@
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="6" t="s">
         <v>36</v>
       </c>
@@ -2183,7 +2192,7 @@
       <c r="G48" s="18"/>
       <c r="H48" s="47"/>
     </row>
-    <row r="49" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
         <v>36</v>
       </c>
@@ -2198,7 +2207,7 @@
       <c r="G49" s="18"/>
       <c r="H49" s="18"/>
     </row>
-    <row r="50" spans="2:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:13" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
         <v>37</v>
       </c>
@@ -2213,7 +2222,7 @@
       <c r="G50" s="18"/>
       <c r="H50" s="18"/>
     </row>
-    <row r="51" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B51" s="32" t="s">
         <v>57</v>
       </c>
@@ -2228,7 +2237,7 @@
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="36" t="s">
         <v>76</v>
       </c>
@@ -2254,7 +2263,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="50">
         <v>1</v>
       </c>
@@ -2280,7 +2289,7 @@
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="50">
         <v>1</v>
       </c>
@@ -2306,7 +2315,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="50">
         <v>2</v>
       </c>
@@ -2332,7 +2341,7 @@
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="54">
         <v>3</v>
       </c>
@@ -2358,7 +2367,7 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="18" t="s">
         <v>82</v>
       </c>
@@ -2369,7 +2378,7 @@
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B58" s="30" t="s">
         <v>87</v>
       </c>
@@ -2381,7 +2390,7 @@
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="40" t="s">
         <v>71</v>
       </c>
@@ -2395,7 +2404,7 @@
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="6">
         <v>1</v>
       </c>
@@ -2407,7 +2416,7 @@
       <c r="F60" s="46"/>
       <c r="G60" s="47"/>
     </row>
-    <row r="61" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="6">
         <v>2</v>
       </c>
@@ -2419,7 +2428,7 @@
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
     </row>
-    <row r="62" spans="2:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:13" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="8">
         <v>3</v>
       </c>
@@ -2431,11 +2440,11 @@
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
     </row>
-    <row r="63" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C21" r:id="rId1"/>
-    <hyperlink ref="C24" r:id="rId2"/>
+    <hyperlink ref="C21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Proyecto de Clase. Ajuste BBDD
</commit_message>
<xml_diff>
--- a/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
+++ b/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\adsi_n-2395871_g3\assets\docs\Trim3\Trim3_Ev1-ModeloRelacional\Trim3_Ev1_1-Normalización\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7B8861-0980-48AA-8F34-253068C05A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="S.I.W.Ventas" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
   <si>
     <t>admin</t>
   </si>
@@ -437,9 +436,6 @@
     <t>(nn) apellidos_user</t>
   </si>
   <si>
-    <t>(uq) identificacion_user</t>
-  </si>
-  <si>
     <t>CATEGORÍAS</t>
   </si>
   <si>
@@ -494,24 +490,115 @@
     <t xml:space="preserve">No puede haber pedidos solo con el seller. </t>
   </si>
   <si>
-    <t>Un Rol es asignado Muchas personas. Una persona se le asigna Un Rol</t>
-  </si>
-  <si>
-    <t>Alejandra</t>
-  </si>
-  <si>
-    <t>Martínez</t>
-  </si>
-  <si>
     <t>profealbeiro2020@</t>
+  </si>
+  <si>
+    <t>customer-2</t>
+  </si>
+  <si>
+    <t>ezequiel@</t>
+  </si>
+  <si>
+    <t>camilo@</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Un</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Usuario se le asigna </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Un</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Rol</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Un</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Rol es asignado a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Muchos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Usuarios</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -545,7 +632,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,14 +651,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -909,21 +990,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -932,9 +1004,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -970,9 +1042,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1057,16 +1126,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1141,29 +1210,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1446,56 +1503,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="10" customWidth="1"/>
-    <col min="2" max="6" width="25.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="46" customWidth="1"/>
-    <col min="8" max="8" width="1.6640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="1.6640625" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="10" customWidth="1"/>
+    <col min="2" max="6" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="45" customWidth="1"/>
+    <col min="8" max="8" width="1.7109375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+    <row r="1" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="33"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>1</v>
       </c>
@@ -1504,295 +1561,289 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="75" t="s">
+    <row r="9" spans="1:10" s="16" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="62"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="63"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="61"/>
       <c r="I10" s="3"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1">
-        <v>123456</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="59"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="62"/>
       <c r="I11" s="3"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="73">
-        <v>3</v>
-      </c>
-      <c r="C12" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="77">
-        <v>654321</v>
-      </c>
-      <c r="E12" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="59"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="58"/>
       <c r="I12" s="3"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="1">
-        <v>987654</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="59"/>
+      <c r="F13" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="58"/>
       <c r="I13" s="3"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="4">
-        <v>654789</v>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="59"/>
+        <v>6</v>
+      </c>
+      <c r="F14" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="58"/>
       <c r="I14" s="3"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="6">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="1">
-        <v>147852</v>
+      <c r="C15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="59"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="58"/>
       <c r="I15" s="3"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="29">
-        <v>1</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="13">
-        <v>456987</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="14" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
         <v>2</v>
       </c>
-      <c r="G16" s="59"/>
+      <c r="C16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="58"/>
       <c r="I16" s="3"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="70">
-        <v>4</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="71">
-        <v>555333</v>
-      </c>
-      <c r="E17" s="71" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="59"/>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="58"/>
       <c r="I17" s="3"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="2:11" s="18" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="32" t="s">
+    <row r="18" spans="2:11" s="17" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="F19"/>
       <c r="G19" s="10"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="36" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="14"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="49" t="s">
-        <v>108</v>
+      <c r="C21" s="48" t="s">
+        <v>104</v>
       </c>
       <c r="D21" s="7">
         <v>12345</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="14"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="48" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="7">
         <v>12345</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="14"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="48" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="7">
         <v>12345</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="14"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
         <v>17</v>
       </c>
@@ -1802,55 +1853,55 @@
       <c r="D24" s="9">
         <v>12345</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="14"/>
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+    <row r="25" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
       <c r="F25"/>
       <c r="G25" s="10"/>
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="32" t="s">
+    <row r="26" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="36" t="s">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="36" t="s">
         <v>25</v>
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="21">
+        <v>96</v>
+      </c>
+      <c r="C28" s="20">
         <v>44788</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -1858,29 +1909,29 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="21">
+        <v>97</v>
+      </c>
+      <c r="C29" s="20">
         <v>44800</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="28" t="s">
+      <c r="D29" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="27" t="s">
         <v>27</v>
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="21">
+        <v>97</v>
+      </c>
+      <c r="C30" s="20">
         <v>44800</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -1888,29 +1939,29 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="26">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="25">
         <v>44804</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>27</v>
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="25">
+        <v>93</v>
+      </c>
+      <c r="C32" s="24">
         <v>44800</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="23" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="9" t="s">
@@ -1918,266 +1969,266 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="18" t="s">
+    <row r="33" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="20"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="19"/>
       <c r="F33"/>
       <c r="G33" s="10"/>
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="34"/>
+    <row r="34" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="33"/>
       <c r="D34" s="3"/>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="40" t="s">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="34" t="s">
         <v>39</v>
       </c>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="G36" s="47"/>
+      <c r="G36" s="46"/>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="G37" s="18"/>
+        <v>89</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="G37" s="17"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E38" s="16"/>
-      <c r="G38" s="18"/>
+        <v>95</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="G38" s="17"/>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="32" t="s">
+    <row r="39" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="62"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="61"/>
       <c r="H39" s="2"/>
       <c r="I39" s="10"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B40" s="36" t="s">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="39" t="s">
+      <c r="D40" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="39" t="s">
+      <c r="E40" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="37" t="s">
+      <c r="F40" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="34" t="s">
         <v>51</v>
       </c>
       <c r="I40" s="10"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="21">
+      <c r="C41" s="20">
         <v>44774</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="42">
         <v>520000</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="42">
         <f>D41*19%</f>
         <v>98800</v>
       </c>
-      <c r="F41" s="42">
+      <c r="F41" s="41">
         <f>D41+E41</f>
         <v>618800</v>
       </c>
-      <c r="G41" s="16" t="s">
+      <c r="G41" s="15" t="s">
         <v>52</v>
       </c>
       <c r="I41" s="10"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="20">
         <v>44774</v>
       </c>
-      <c r="D42" s="43">
+      <c r="D42" s="42">
         <v>150000</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="42">
         <f t="shared" ref="E42:E44" si="0">D42*19%</f>
         <v>28500</v>
       </c>
-      <c r="F42" s="42">
+      <c r="F42" s="41">
         <f t="shared" ref="F42:F44" si="1">D42+E42</f>
         <v>178500</v>
       </c>
-      <c r="G42" s="68" t="s">
+      <c r="G42" s="67" t="s">
         <v>78</v>
       </c>
       <c r="I42" s="10"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="21">
+      <c r="C43" s="20">
         <v>44803</v>
       </c>
-      <c r="D43" s="43">
+      <c r="D43" s="42">
         <v>230000</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="42">
         <f t="shared" si="0"/>
         <v>43700</v>
       </c>
-      <c r="F43" s="42">
+      <c r="F43" s="41">
         <f t="shared" si="1"/>
         <v>273700</v>
       </c>
-      <c r="G43" s="69" t="s">
+      <c r="G43" s="68" t="s">
         <v>79</v>
       </c>
       <c r="I43" s="10"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="25">
+      <c r="C44" s="24">
         <v>44819</v>
       </c>
-      <c r="D44" s="44">
+      <c r="D44" s="43">
         <v>80000</v>
       </c>
-      <c r="E44" s="44">
+      <c r="E44" s="43">
         <f t="shared" si="0"/>
         <v>15200</v>
       </c>
-      <c r="F44" s="45">
+      <c r="F44" s="44">
         <f t="shared" si="1"/>
         <v>95200</v>
       </c>
-      <c r="G44" s="69" t="s">
+      <c r="G44" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="H44" s="16"/>
+      <c r="H44" s="15"/>
       <c r="I44" s="10"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="18" t="s">
+    <row r="45" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="20"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="19"/>
       <c r="F45"/>
-      <c r="G45" s="15"/>
+      <c r="G45" s="14"/>
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" s="33"/>
-      <c r="D46" s="34"/>
+    <row r="46" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="32"/>
+      <c r="D46" s="33"/>
       <c r="E46" s="3"/>
-      <c r="G46" s="18"/>
+      <c r="G46" s="17"/>
       <c r="H46" s="2"/>
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B47" s="40" t="s">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="67" t="s">
+      <c r="C47" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="41" t="s">
+      <c r="D47" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="35"/>
-      <c r="G47" s="18"/>
+      <c r="E47" s="34"/>
+      <c r="G47" s="17"/>
       <c r="H47" s="2"/>
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>36</v>
       </c>
@@ -2187,12 +2238,12 @@
       <c r="D48" s="7">
         <v>5</v>
       </c>
-      <c r="E48" s="18"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="47"/>
-    </row>
-    <row r="49" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="17"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="46"/>
+    </row>
+    <row r="49" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
         <v>36</v>
       </c>
@@ -2202,252 +2253,258 @@
       <c r="D49" s="7">
         <v>1</v>
       </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-    </row>
-    <row r="50" spans="2:13" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="2:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="48" t="s">
+      <c r="C50" s="47" t="s">
         <v>54</v>
       </c>
       <c r="D50" s="9">
         <v>3</v>
       </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-    </row>
-    <row r="51" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="32" t="s">
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="62"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="61"/>
       <c r="J51" s="10"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B52" s="36" t="s">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="64" t="s">
+      <c r="C52" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="38" t="s">
+      <c r="D52" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E52" s="39" t="s">
+      <c r="E52" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="F52" s="39" t="s">
+      <c r="F52" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G52" s="37" t="s">
+      <c r="G52" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="H52" s="63"/>
+      <c r="H52" s="62"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B53" s="50">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" s="49">
         <v>1</v>
       </c>
-      <c r="C53" s="65" t="s">
+      <c r="C53" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="51" t="s">
+      <c r="D53" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="E53" s="52">
+      <c r="E53" s="51">
         <v>2500</v>
       </c>
-      <c r="F53" s="52">
+      <c r="F53" s="51">
         <v>1</v>
       </c>
-      <c r="G53" s="58" t="s">
+      <c r="G53" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H53" s="60"/>
+      <c r="H53" s="59"/>
       <c r="I53" s="10"/>
       <c r="J53" s="10"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B54" s="50">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="49">
         <v>1</v>
       </c>
-      <c r="C54" s="65" t="s">
+      <c r="C54" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="51" t="s">
+      <c r="D54" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="E54" s="52">
+      <c r="E54" s="51">
         <v>6500</v>
       </c>
-      <c r="F54" s="52">
+      <c r="F54" s="51">
         <v>1</v>
       </c>
-      <c r="G54" s="53" t="s">
+      <c r="G54" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="H54" s="61"/>
+      <c r="H54" s="60"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B55" s="50">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="49">
         <v>2</v>
       </c>
-      <c r="C55" s="65" t="s">
+      <c r="C55" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="51" t="s">
+      <c r="D55" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E55" s="52">
+      <c r="E55" s="51">
         <v>3500</v>
       </c>
-      <c r="F55" s="52">
+      <c r="F55" s="51">
         <v>1</v>
       </c>
-      <c r="G55" s="53" t="s">
+      <c r="G55" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="H55" s="61"/>
+      <c r="H55" s="60"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="54">
+    <row r="56" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="53">
         <v>3</v>
       </c>
-      <c r="C56" s="66" t="s">
+      <c r="C56" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="D56" s="55" t="s">
+      <c r="D56" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="E56" s="56">
+      <c r="E56" s="55">
         <v>4500</v>
       </c>
-      <c r="F56" s="56">
+      <c r="F56" s="55">
         <v>250</v>
       </c>
-      <c r="G56" s="57" t="s">
+      <c r="G56" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="H56" s="61"/>
-      <c r="I56" s="16"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="15"/>
       <c r="J56" s="10"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="18" t="s">
+    <row r="57" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="20"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="19"/>
       <c r="F57"/>
       <c r="G57" s="10"/>
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58" s="31"/>
+    <row r="58" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="30"/>
       <c r="D58" s="3"/>
-      <c r="F58" s="46"/>
+      <c r="F58" s="45"/>
       <c r="G58" s="2"/>
       <c r="H58"/>
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B59" s="40" t="s">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B59" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C59" s="41" t="s">
+      <c r="C59" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="35"/>
-      <c r="F59" s="46"/>
+      <c r="D59" s="34"/>
+      <c r="F59" s="45"/>
       <c r="G59" s="2"/>
       <c r="H59"/>
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="6">
         <v>1</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="47"/>
-    </row>
-    <row r="61" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="17"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="46"/>
+    </row>
+    <row r="61" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="6">
         <v>2</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-    </row>
-    <row r="62" spans="2:13" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+    </row>
+    <row r="62" spans="2:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="8">
         <v>3</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-    </row>
-    <row r="63" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+    </row>
+    <row r="63" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C21" r:id="rId1"/>
+    <hyperlink ref="C24" r:id="rId2"/>
+    <hyperlink ref="F12" r:id="rId3"/>
+    <hyperlink ref="F13" r:id="rId4"/>
+    <hyperlink ref="F14" r:id="rId5"/>
+    <hyperlink ref="F17" r:id="rId6"/>
+    <hyperlink ref="F15" r:id="rId7"/>
+    <hyperlink ref="F16" r:id="rId8"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="60" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup scale="60" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proyecto de Clase. BBDD - Consultas en Una Tabla
</commit_message>
<xml_diff>
--- a/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
+++ b/assets/docs/Trim3/Trim3_Ev1-ModeloRelacional/Trim3_Ev1_1-Normalización/Trim3_Ev1_1-Normalización_MER.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="119">
   <si>
     <t>admin</t>
   </si>
@@ -668,13 +668,312 @@
   </si>
   <si>
     <t>(nn) fecha_ingreso_cred</t>
+  </si>
+  <si>
+    <t>admin-2</t>
+  </si>
+  <si>
+    <t>Pepito</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>jorge@</t>
+  </si>
+  <si>
+    <t>Devolución Dinero</t>
+  </si>
+  <si>
+    <t>CATEGORIAS</t>
+  </si>
+  <si>
+    <t>PRODUCTOS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Una</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Categoría</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pertenecen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Muchos </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Productos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Un </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Producto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pertenece</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Una</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Categoría</t>
+    </r>
+  </si>
+  <si>
+    <t>(pk) codigo_categoria</t>
+  </si>
+  <si>
+    <t>(nn) nombre_categoria</t>
+  </si>
+  <si>
+    <t>(fk) codigo_producto</t>
+  </si>
+  <si>
+    <t>(nn) nombre_producto</t>
+  </si>
+  <si>
+    <t>(fk) codigo_categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(nn) precio_categoria </t>
+  </si>
+  <si>
+    <t>(nn) unidad_producto</t>
+  </si>
+  <si>
+    <t>(nn) medida_producto</t>
+  </si>
+  <si>
+    <t>producto-1</t>
+  </si>
+  <si>
+    <t>producto-2</t>
+  </si>
+  <si>
+    <t>producto-3</t>
+  </si>
+  <si>
+    <t>producto-4</t>
+  </si>
+  <si>
+    <t>producto-5</t>
+  </si>
+  <si>
+    <t>producto-6</t>
+  </si>
+  <si>
+    <t>producto-7</t>
+  </si>
+  <si>
+    <t>producto-8</t>
+  </si>
+  <si>
+    <t>producto-9</t>
+  </si>
+  <si>
+    <t>producto-10</t>
+  </si>
+  <si>
+    <t>producto-11</t>
+  </si>
+  <si>
+    <t>producto-12</t>
+  </si>
+  <si>
+    <t>Papa</t>
+  </si>
+  <si>
+    <t>Zanahoria</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>Arroz</t>
+  </si>
+  <si>
+    <t>Aceite</t>
+  </si>
+  <si>
+    <t>Lentejas</t>
+  </si>
+  <si>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Gaseosa</t>
+  </si>
+  <si>
+    <t>Cerveza</t>
+  </si>
+  <si>
+    <t>Jabón Baño</t>
+  </si>
+  <si>
+    <t>Jabón Ropa</t>
+  </si>
+  <si>
+    <t>Shampoo</t>
+  </si>
+  <si>
+    <t>libra</t>
+  </si>
+  <si>
+    <t>gramos</t>
+  </si>
+  <si>
+    <t>litro</t>
+  </si>
+  <si>
+    <t>botella</t>
+  </si>
+  <si>
+    <t>mililitros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,6 +1035,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1025,11 +1331,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1198,9 +1505,40 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1479,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,13 +2096,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
-      <c r="C20" s="32">
+      <c r="C20" s="41">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1778,292 +2116,278 @@
       <c r="J20" s="36"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
-      <c r="C21" s="34">
+      <c r="C21" s="32">
         <v>3</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="43" t="s">
-        <v>9</v>
+      <c r="G21" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>
       <c r="J21" s="36"/>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="36"/>
+      <c r="C22" s="34">
+        <v>1</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>9</v>
+      </c>
       <c r="H22" s="36"/>
       <c r="I22" s="36"/>
       <c r="J22" s="36"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="27" t="s">
+    <row r="23" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="25"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="C24" s="28" t="s">
+      <c r="D24" s="8"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="25"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="C25" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="29"/>
-      <c r="K24" s="24"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="C25" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>22</v>
-      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="29"/>
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
-      <c r="C26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="9">
-        <v>44788</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>24</v>
+      <c r="C26" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>22</v>
       </c>
       <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="C27" s="32" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D27" s="9">
-        <v>44800</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="45" t="s">
-        <v>63</v>
+        <v>44788</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>24</v>
       </c>
       <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="C28" s="32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D28" s="9">
         <v>44800</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>63</v>
       </c>
       <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="9">
+        <v>44800</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="C30" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D30" s="12">
         <v>44804</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E30" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="47" t="s">
+      <c r="F30" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="24"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="C30" s="48" t="s">
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="C31" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="49">
+      <c r="D31" s="12">
         <v>44805</v>
       </c>
-      <c r="E30" s="50" t="s">
+      <c r="E31" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F31" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="24"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="19"/>
       <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="1:11" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="25"/>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="C32" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="49">
+        <v>44836</v>
+      </c>
+      <c r="E32" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="51"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="19"/>
+      <c r="K33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="25"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="C35" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="25"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="C34" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="J34" s="21"/>
-      <c r="K34" s="25"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="C35" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="1">
-        <v>123456</v>
-      </c>
-      <c r="E35" s="9">
-        <v>44723</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H35" s="1">
-        <v>12345</v>
-      </c>
-      <c r="I35" s="33">
-        <v>1</v>
-      </c>
-      <c r="J35" s="19"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="20"/>
       <c r="K35" s="25"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
-      <c r="C36" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="1">
-        <v>456789</v>
-      </c>
-      <c r="E36" s="9">
-        <v>44754</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H36" s="1">
-        <v>12345</v>
-      </c>
-      <c r="I36" s="33">
-        <v>0</v>
-      </c>
-      <c r="J36" s="19"/>
+      <c r="C36" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="21"/>
       <c r="K36" s="25"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="C37" s="32" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D37" s="1">
-        <v>987654</v>
+        <v>123456</v>
       </c>
       <c r="E37" s="9">
-        <v>44786</v>
+        <v>44723</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H37" s="1">
         <v>12345</v>
@@ -2074,137 +2398,521 @@
       <c r="J37" s="19"/>
       <c r="K37" s="25"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
-      <c r="C38" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="53">
-        <v>654321</v>
-      </c>
-      <c r="E38" s="49">
-        <v>44801</v>
-      </c>
-      <c r="F38" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="G38" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="H38" s="53">
+      <c r="C38" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="1">
+        <v>456789</v>
+      </c>
+      <c r="E38" s="9">
+        <v>44754</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="1">
         <v>12345</v>
       </c>
-      <c r="I38" s="35">
+      <c r="I38" s="33">
         <v>0</v>
       </c>
       <c r="J38" s="19"/>
       <c r="K38" s="25"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
+      <c r="C39" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="1">
+        <v>987654</v>
+      </c>
+      <c r="E39" s="9">
+        <v>44786</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" s="1">
+        <v>12345</v>
+      </c>
+      <c r="I39" s="33">
+        <v>1</v>
+      </c>
+      <c r="J39" s="19"/>
       <c r="K39" s="25"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24"/>
-      <c r="K40" s="24"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C40" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="53">
+        <v>654321</v>
+      </c>
+      <c r="E40" s="49">
+        <v>44801</v>
+      </c>
+      <c r="F40" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" s="53">
+        <v>12345</v>
+      </c>
+      <c r="I40" s="35">
+        <v>0</v>
+      </c>
+      <c r="J40" s="19"/>
+      <c r="K40" s="25"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
-      <c r="K41" s="24"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="K42" s="24"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="25"/>
+    </row>
+    <row r="42" spans="1:11" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="25"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="25"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
+      <c r="C43" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="29"/>
       <c r="K43" s="24"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="24"/>
+      <c r="C44" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>83</v>
+      </c>
       <c r="K44" s="24"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="24"/>
+      <c r="C45" s="32">
+        <v>1</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>0</v>
+      </c>
       <c r="K45" s="24"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="24"/>
+      <c r="C46" s="32">
+        <v>2</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="K46" s="24"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
+      <c r="C47" s="32">
+        <v>3</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>36</v>
+      </c>
       <c r="K47" s="24"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24"/>
+      <c r="C48" s="34">
+        <v>4</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>37</v>
+      </c>
       <c r="K48" s="24"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24"/>
       <c r="K49" s="24"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="K50" s="24"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="25"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="25"/>
+    </row>
+    <row r="51" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
-      <c r="K51" s="24"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C51" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="2"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="24"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
-      <c r="K52" s="24"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C52" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="I52" s="2"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="24"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
-      <c r="K53" s="24"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C53" s="32">
+        <v>1</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="F53" s="65">
+        <v>950.3</v>
+      </c>
+      <c r="G53" s="58">
+        <v>1</v>
+      </c>
+      <c r="H53" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I53" s="2"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="24"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
-      <c r="K54" s="24"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C54" s="32">
+        <v>1</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="F54" s="65">
+        <v>630.33000000000004</v>
+      </c>
+      <c r="G54" s="58">
+        <v>1</v>
+      </c>
+      <c r="H54" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="24"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="24"/>
-      <c r="K55" s="24"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C55" s="32">
+        <v>1</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="65">
+        <v>750.55</v>
+      </c>
+      <c r="G55" s="58">
+        <v>1</v>
+      </c>
+      <c r="H55" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="24"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="24"/>
-      <c r="K56" s="24"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C56" s="46">
+        <v>2</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="F56" s="66">
+        <v>2500</v>
+      </c>
+      <c r="G56" s="61">
+        <v>500</v>
+      </c>
+      <c r="H56" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="24"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
-      <c r="K57" s="24"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C57" s="46">
+        <v>2</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="F57" s="66">
+        <v>10500</v>
+      </c>
+      <c r="G57" s="61">
+        <v>1</v>
+      </c>
+      <c r="H57" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="24"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="24"/>
-      <c r="K58" s="24"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C58" s="46">
+        <v>2</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="66">
+        <v>3500</v>
+      </c>
+      <c r="G58" s="61">
+        <v>1000</v>
+      </c>
+      <c r="H58" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="24"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
-      <c r="K59" s="24"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C59" s="32">
+        <v>3</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="F59" s="65">
+        <v>3000</v>
+      </c>
+      <c r="G59" s="58">
+        <v>1.5</v>
+      </c>
+      <c r="H59" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="I59" s="2"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="24"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
-      <c r="K60" s="24"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="32">
+        <v>3</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="F60" s="65">
+        <v>3500</v>
+      </c>
+      <c r="G60" s="58">
+        <v>2.5</v>
+      </c>
+      <c r="H60" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="I60" s="2"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="24"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
-      <c r="K61" s="24"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C61" s="32">
+        <v>3</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="F61" s="65">
+        <v>2500</v>
+      </c>
+      <c r="G61" s="58">
+        <v>1</v>
+      </c>
+      <c r="H61" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="I61" s="2"/>
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="24"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
-      <c r="K62" s="24"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C62" s="46">
+        <v>4</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E62" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F62" s="66">
+        <v>1200</v>
+      </c>
+      <c r="G62" s="61">
+        <v>285</v>
+      </c>
+      <c r="H62" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="I62" s="2"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="24"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
-      <c r="K63" s="24"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C63" s="46">
+        <v>4</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E63" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="F63" s="66">
+        <v>12000</v>
+      </c>
+      <c r="G63" s="61">
+        <v>1000</v>
+      </c>
+      <c r="H63" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="I63" s="2"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="24"/>
+    </row>
+    <row r="64" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24"/>
-      <c r="K64" s="24"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C64" s="48">
+        <v>4</v>
+      </c>
+      <c r="D64" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="E64" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="F64" s="67">
+        <v>18500</v>
+      </c>
+      <c r="G64" s="63">
+        <v>750</v>
+      </c>
+      <c r="H64" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="I64" s="2"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="24"/>
+    </row>
+    <row r="65" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24"/>
       <c r="K65" s="24"/>
     </row>
@@ -2340,27 +3048,59 @@
       <c r="A98" s="24"/>
       <c r="K98" s="24"/>
     </row>
-    <row r="99" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="24"/>
-      <c r="B99" s="24"/>
-      <c r="C99" s="26"/>
-      <c r="D99" s="26"/>
-      <c r="E99" s="26"/>
-      <c r="F99" s="26"/>
-      <c r="G99" s="26"/>
-      <c r="H99" s="26"/>
-      <c r="I99" s="26"/>
-      <c r="J99" s="26"/>
       <c r="K99" s="24"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="24"/>
+      <c r="K100" s="24"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="24"/>
+      <c r="K101" s="24"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="24"/>
+      <c r="K102" s="24"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="24"/>
+      <c r="K103" s="24"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="24"/>
+      <c r="K104" s="24"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="24"/>
+      <c r="K105" s="24"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="24"/>
+      <c r="K106" s="24"/>
+    </row>
+    <row r="107" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="24"/>
+      <c r="B107" s="24"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="26"/>
+      <c r="G107" s="26"/>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="26"/>
+      <c r="K107" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G16" r:id="rId1"/>
     <hyperlink ref="G17" r:id="rId2"/>
     <hyperlink ref="G18" r:id="rId3"/>
-    <hyperlink ref="G21" r:id="rId4"/>
+    <hyperlink ref="G22" r:id="rId4"/>
     <hyperlink ref="G19" r:id="rId5"/>
-    <hyperlink ref="G20" r:id="rId6"/>
+    <hyperlink ref="G21" r:id="rId6"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>